<commit_message>
ordered todo list by importance
</commit_message>
<xml_diff>
--- a/Todo.xlsx
+++ b/Todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>mögliche Rücksendung:</t>
   </si>
@@ -46,18 +46,12 @@
     <t>zwei Schaltungen fertig bauen</t>
   </si>
   <si>
-    <t>zwei Boxen fertig bauen</t>
-  </si>
-  <si>
     <t>Module testen</t>
   </si>
   <si>
     <t>eventuell Box für Lampignon</t>
   </si>
   <si>
-    <t>Hütchen für Lampignon</t>
-  </si>
-  <si>
     <t>neuronale Netze noch mal testen</t>
   </si>
   <si>
@@ -74,13 +68,25 @@
   </si>
   <si>
     <t>eventuell neuronale Netze unter Verwendung des Handschuhs konstruieren</t>
+  </si>
+  <si>
+    <t>Hütchen für Lampignon berechnen und entwerfen</t>
+  </si>
+  <si>
+    <t>mit Marcel über die Bestellungen reden</t>
+  </si>
+  <si>
+    <t>zwei Boxen mit CAD erstellen und drucken</t>
+  </si>
+  <si>
+    <t>Hütchen für Lampignon mit CAD erstellen und drucken</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,13 +94,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,13 +148,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,112 +466,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A27"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>